<commit_message>
update "Absenz erstellen" and trained model f - fixed from and to date bug
</commit_message>
<xml_diff>
--- a/import/datastore/Absences.xlsx
+++ b/import/datastore/Absences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5320" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="66">
   <si>
     <t>ski</t>
   </si>
@@ -183,21 +183,6 @@
     <t>brm</t>
   </si>
   <si>
-    <t>2017-07-15</t>
-  </si>
-  <si>
-    <t>2017-07-22</t>
-  </si>
-  <si>
-    <t>2017-07-31</t>
-  </si>
-  <si>
-    <t>2017-08-06</t>
-  </si>
-  <si>
-    <t>Weiterbildung</t>
-  </si>
-  <si>
     <t>2017-02-15</t>
   </si>
   <si>
@@ -213,19 +198,37 @@
     <t>false</t>
   </si>
   <si>
-    <t>2017-05-15</t>
-  </si>
-  <si>
-    <t>Umzug</t>
-  </si>
-  <si>
-    <t>2017-05-16</t>
-  </si>
-  <si>
     <t>Vaterschaftsurlaub</t>
   </si>
   <si>
     <t>2017-05-13</t>
+  </si>
+  <si>
+    <t>Kurs</t>
+  </si>
+  <si>
+    <t>2017-03-22</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Krankheit</t>
+  </si>
+  <si>
+    <t>emploji</t>
+  </si>
+  <si>
+    <t>2017-03-15</t>
+  </si>
+  <si>
+    <t>2017-05-02</t>
+  </si>
+  <si>
+    <t>2017-05-19</t>
+  </si>
+  <si>
+    <t>Wohnungswechsel</t>
   </si>
 </sst>
 </file>
@@ -327,7 +330,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -411,6 +414,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -426,7 +430,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="84">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -499,6 +503,7 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -567,7 +572,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -622,7 +627,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -677,7 +682,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -734,7 +739,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -791,7 +796,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -848,7 +853,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -903,7 +908,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -960,7 +965,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1015,7 +1020,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1072,7 +1077,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1129,7 +1134,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1186,7 +1191,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1241,7 +1246,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1298,7 +1303,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1353,7 +1358,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1408,7 +1413,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1463,7 +1468,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1520,7 +1525,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1575,7 +1580,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1630,7 +1635,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1687,7 +1692,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1742,7 +1747,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1797,7 +1802,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1854,7 +1859,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1911,7 +1916,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1968,7 +1973,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2023,7 +2028,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2080,7 +2085,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2135,7 +2140,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2190,7 +2195,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2245,7 +2250,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2302,7 +2307,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2357,7 +2362,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2412,7 +2417,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2469,7 +2474,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2524,7 +2529,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2579,7 +2584,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2636,7 +2641,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2693,7 +2698,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2750,7 +2755,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3088,8 +3093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3215,7 +3220,7 @@
         <v>36</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -3278,19 +3283,19 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="M5" t="str">
         <f>"{"</f>
@@ -3302,51 +3307,51 @@
       </c>
       <c r="O5" t="str">
         <f t="shared" ref="O5:Y5" si="2">IF(O$4=0,N5,N5&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B5&amp;"""",IF(O$3=2,IF(B5=1,"true", "false"),B5))&amp;IF(ISBLANK(P$3),"},",""))</f>
-        <v>{"user":"brm","typ":"Weiterbildung"</v>
+        <v>{"user":"brm","typ":"Kurs"</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":""</v>
+        <v>{"user":"brm","typ":"Kurs","text":""</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15"</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z5" t="str">
         <f>IF(ISBLANK(A5),"",Y5&amp;"}"&amp;IF(OR(Z6="]",Z6="",ISBLANK(Z6)),"",","))</f>
-        <v>{"user":"brm","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
+        <v>{"user":"brm","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -3357,16 +3362,16 @@
         <v>31</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" ref="M6:M55" si="3">"{"</f>
@@ -3386,43 +3391,43 @@
       </c>
       <c r="Q6" t="str">
         <f t="shared" ref="Q6:Q55" si="7">IF(Q$4=0,P6,P6&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D6&amp;"""",IF(Q$3=2,IF(D6=1,"true", "false"),D6))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15"</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" ref="R6:R55" si="8">IF(R$4=0,Q6,Q6&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E6&amp;"""",IF(R$3=2,IF(E6=1,"true", "false"),E6))&amp;IF(ISBLANK(S$3),"},",""))</f>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22"</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" ref="S6:S55" si="9">IF(S$4=0,R6,R6&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F6&amp;"""",IF(S$3=2,IF(F6=1,"true", "false"),F6))&amp;IF(ISBLANK(T$3),"},",""))</f>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T6" t="str">
         <f t="shared" ref="T6:T55" si="10">IF(T$4=0,S6,S6&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G6&amp;"""",IF(T$3=2,IF(G6=1,"true", "false"),G6))&amp;IF(ISBLANK(U$3),"},",""))</f>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ref="U6:Y55" si="11">IF(U$4=0,T6,T6&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H6&amp;"""",IF(U$3=2,IF(H6=1,"true", "false"),H6))&amp;IF(ISBLANK(V$3),"},",""))</f>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Y6" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ref="Z6:Z55" si="12">IF(ISBLANK(A6),"",Y6&amp;"}"&amp;IF(OR(Z7="]",Z7="",ISBLANK(Z7)),"",","))</f>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false},</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -3433,16 +3438,16 @@
         <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="3"/>
@@ -3462,43 +3467,43 @@
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31"</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06"</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14</v>
       </c>
       <c r="T7" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="U7" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="X7" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false},</v>
+        <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false},</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -3506,19 +3511,19 @@
         <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="3"/>
@@ -3530,51 +3535,51 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"cogji","typ":"Weiterbildung"</v>
+        <v>{"user":"cogji","typ":"Kurs"</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":""</v>
+        <v>{"user":"cogji","typ":"Kurs","text":""</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15"</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"cogji","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
+        <v>{"user":"cogji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -3585,16 +3590,16 @@
         <v>31</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="3"/>
@@ -3614,43 +3619,43 @@
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15"</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22"</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="U9" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="X9" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Y9" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false},</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -3661,16 +3666,16 @@
         <v>31</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="3"/>
@@ -3690,43 +3695,43 @@
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31"</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06"</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14</v>
       </c>
       <c r="T10" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false},</v>
+        <v>{"user":"cogji","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false},</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -3734,19 +3739,19 @@
         <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="3"/>
@@ -3758,51 +3763,51 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"david","typ":"Weiterbildung"</v>
+        <v>{"user":"david","typ":"Kurs"</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":""</v>
+        <v>{"user":"david","typ":"Kurs","text":""</v>
       </c>
       <c r="Q11" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15"</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T11" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X11" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y11" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"david","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
+        <v>{"user":"david","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -3813,16 +3818,16 @@
         <v>31</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F12">
         <v>5</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="3"/>
@@ -3842,43 +3847,43 @@
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15"</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22"</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T12" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="U12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Y12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false},</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
@@ -3889,16 +3894,16 @@
         <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="3"/>
@@ -3918,43 +3923,43 @@
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31"</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06"</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false},</v>
+        <v>{"user":"david","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false},</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -3962,19 +3967,19 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F14">
         <v>19</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="3"/>
@@ -4038,9 +4043,9 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -4050,7 +4055,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="3"/>
@@ -4062,51 +4067,51 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien"</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit"</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":""</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":""</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15"</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22"</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":5</v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":5,"commit":false</v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":5,"commit":false</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":5,"commit":false</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":5,"commit":false</v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":5,"commit":false</v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":5,"commit":false</v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false},</v>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -4117,16 +4122,16 @@
         <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F16">
         <v>5</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="3"/>
@@ -4146,43 +4151,43 @@
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31"</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06"</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":5</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":5,"commit":false</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":5,"commit":false</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":5,"commit":false</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":5,"commit":false</v>
       </c>
       <c r="X16" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":5,"commit":false</v>
       </c>
       <c r="Y16" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":5,"commit":false</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="12"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false},</v>
+        <f>IF(ISBLANK(A16),"",Y16&amp;"}"&amp;IF(OR(Z17="]",Z17="",ISBLANK(Z17)),"",","))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
@@ -4190,19 +4195,19 @@
         <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F17">
         <v>3</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="3"/>
@@ -4214,51 +4219,51 @@
       </c>
       <c r="O17" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung"</v>
+        <v>{"user":"meyerchri","typ":"Kurs"</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":""</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":""</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15"</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T17" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U17" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X17" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y17" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"meyerchri","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
+        <v>{"user":"meyerchri","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
@@ -4266,19 +4271,19 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="10" t="s">
         <v>62</v>
       </c>
+      <c r="E18" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="F18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="3"/>
@@ -4290,51 +4295,51 @@
       </c>
       <c r="O18" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"meyerchri","typ":"Umzug"</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel"</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":""</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":""</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15"</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16"</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16","days":2</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T18" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16","days":2,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":true</v>
       </c>
       <c r="U18" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16","days":2,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":true</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16","days":2,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":true</v>
       </c>
       <c r="W18" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16","days":2,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":true</v>
       </c>
       <c r="X18" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16","days":2,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":true</v>
       </c>
       <c r="Y18" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16","days":2,"commit":true</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":true</v>
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"meyerchri","typ":"Umzug","text":"","fromDate":"2017-05-15","toDate":"2017-05-16","days":2,"commit":true},</v>
+        <v>{"user":"meyerchri","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":true},</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
@@ -4345,16 +4350,16 @@
         <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="3"/>
@@ -4374,43 +4379,43 @@
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31"</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06"</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14</v>
       </c>
       <c r="T19" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="U19" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="W19" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="X19" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Y19" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false},</v>
+        <v>{"user":"meyerchri","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false},</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
@@ -4418,19 +4423,19 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F20">
         <v>3</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="3"/>
@@ -4442,51 +4447,51 @@
       </c>
       <c r="O20" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung"</v>
+        <v>{"user":"remostrupler","typ":"Kurs"</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":""</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":""</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15"</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R20" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T20" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U20" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W20" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X20" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y20" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"remostrupler","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
+        <v>{"user":"remostrupler","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
@@ -4497,16 +4502,16 @@
         <v>31</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F21">
         <v>5</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="3"/>
@@ -4526,43 +4531,43 @@
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15"</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R21" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22"</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T21" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="W21" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="X21" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Y21" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false},</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
@@ -4573,16 +4578,16 @@
         <v>31</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="3"/>
@@ -4602,43 +4607,43 @@
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31"</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R22" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06"</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14</v>
       </c>
       <c r="T22" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="U22" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="W22" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="X22" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Y22" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Z22" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false},</v>
+        <v>{"user":"remostrupler","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false},</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
@@ -4646,19 +4651,19 @@
         <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F23">
         <v>3</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="3"/>
@@ -4670,51 +4675,51 @@
       </c>
       <c r="O23" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung"</v>
+        <v>{"user":"susanne_s","typ":"Kurs"</v>
       </c>
       <c r="P23" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":""</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":""</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15"</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R23" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T23" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U23" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V23" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W23" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X23" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y23" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z23" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"susanne_s","typ":"Weiterbildung","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
+        <v>{"user":"susanne_s","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
@@ -4725,16 +4730,16 @@
         <v>31</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F24">
         <v>5</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="3"/>
@@ -4754,43 +4759,43 @@
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15"</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R24" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22"</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T24" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="U24" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="V24" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="W24" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="X24" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Y24" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Z24" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-15","toDate":"2017-07-22","days":5,"commit":false},</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
@@ -4801,16 +4806,16 @@
         <v>31</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F25">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="3"/>
@@ -4830,449 +4835,575 @@
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31"</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R25" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06"</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S25" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14</v>
       </c>
       <c r="T25" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="U25" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="V25" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="W25" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="X25" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Y25" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Z25" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-07-31","toDate":"2017-08-06","days":5,"commit":false}</v>
+        <v>{"user":"susanne_s","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false},</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M26" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" ref="N26:N28" si="13">IF(N$4=0,M26,M26&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A26&amp;"""",IF(N$3=2,IF(A26=1,"true", "false"),A26))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":"User"</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" ref="O26:O28" si="14">IF(O$4=0,N26,N26&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B26&amp;"""",IF(O$3=2,IF(B26=1,"true", "false"),B26))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs"</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" ref="P26:P28" si="15">IF(P$4=0,O26,O26&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C26&amp;"""",IF(P$3=2,IF(C26=1,"true", "false"),C26))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":""</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" ref="Q26:Q28" si="16">IF(Q$4=0,P26,P26&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D26&amp;"""",IF(Q$3=2,IF(D26=1,"true", "false"),D26))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" ref="R26:R28" si="17">IF(R$4=0,Q26,Q26&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E26&amp;"""",IF(R$3=2,IF(E26=1,"true", "false"),E26))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" ref="S26:S28" si="18">IF(S$4=0,R26,R26&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F26&amp;"""",IF(S$3=2,IF(F26=1,"true", "false"),F26))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="T26:T28" si="19">IF(T$4=0,S26,S26&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G26&amp;"""",IF(T$3=2,IF(G26=1,"true", "false"),G26))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="U26:U28" si="20">IF(U$4=0,T26,T26&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H26&amp;"""",IF(U$3=2,IF(H26=1,"true", "false"),H26))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V26" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="V26:V28" si="21">IF(V$4=0,U26,U26&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I26&amp;"""",IF(V$3=2,IF(I26=1,"true", "false"),I26))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="W26:W28" si="22">IF(W$4=0,V26,V26&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J26&amp;"""",IF(W$3=2,IF(J26=1,"true", "false"),J26))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X26" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="X26:X28" si="23">IF(X$4=0,W26,W26&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K26&amp;"""",IF(X$3=2,IF(K26=1,"true", "false"),K26))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="Y26:Y28" si="24">IF(Y$4=0,X26,X26&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L26&amp;"""",IF(Y$3=2,IF(L26=1,"true", "false"),L26))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" ref="Z26:Z28" si="25">IF(ISBLANK(A26),"",Y26&amp;"}"&amp;IF(OR(Z27="]",Z27="",ISBLANK(Z27)),"",","))</f>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="M27" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="13"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O27" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="14"/>
+        <v>{"user":"User","typ":"Wohnungswechsel"</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="15"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":""</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="16"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="17"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="18"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="19"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="20"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="V27" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="21"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="W27" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="22"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="X27" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="23"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="24"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Z27" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="25"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="M28" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="13"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O28" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="14"/>
+        <v>{"user":"User","typ":"Ferien"</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="15"/>
+        <v>{"user":"User","typ":"Ferien","text":""</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="16"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="17"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="18"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="19"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="20"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="V28" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="21"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="W28" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="22"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="X28" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="23"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Y28" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="24"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Z28" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="25"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false},</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M29" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" ref="N29:N31" si="26">IF(N$4=0,M29,M29&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A29&amp;"""",IF(N$3=2,IF(A29=1,"true", "false"),A29))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":"emploji"</v>
       </c>
       <c r="O29" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" ref="O29:O31" si="27">IF(O$4=0,N29,N29&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B29&amp;"""",IF(O$3=2,IF(B29=1,"true", "false"),B29))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs"</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" ref="P29:P31" si="28">IF(P$4=0,O29,O29&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C29&amp;"""",IF(P$3=2,IF(C29=1,"true", "false"),C29))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":""</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" ref="Q29:Q31" si="29">IF(Q$4=0,P29,P29&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D29&amp;"""",IF(Q$3=2,IF(D29=1,"true", "false"),D29))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R29" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" ref="R29:R31" si="30">IF(R$4=0,Q29,Q29&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E29&amp;"""",IF(R$3=2,IF(E29=1,"true", "false"),E29))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" ref="S29:S31" si="31">IF(S$4=0,R29,R29&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F29&amp;"""",IF(S$3=2,IF(F29=1,"true", "false"),F29))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="T29:T31" si="32">IF(T$4=0,S29,S29&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G29&amp;"""",IF(T$3=2,IF(G29=1,"true", "false"),G29))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="U29:U31" si="33">IF(U$4=0,T29,T29&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H29&amp;"""",IF(U$3=2,IF(H29=1,"true", "false"),H29))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V29" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="V29:V31" si="34">IF(V$4=0,U29,U29&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I29&amp;"""",IF(V$3=2,IF(I29=1,"true", "false"),I29))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W29" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="W29:W31" si="35">IF(W$4=0,V29,V29&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J29&amp;"""",IF(W$3=2,IF(J29=1,"true", "false"),J29))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X29" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="X29:X31" si="36">IF(X$4=0,W29,W29&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K29&amp;"""",IF(X$3=2,IF(K29=1,"true", "false"),K29))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y29" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="Y29:Y31" si="37">IF(Y$4=0,X29,X29&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L29&amp;"""",IF(Y$3=2,IF(L29=1,"true", "false"),L29))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z29" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" ref="Z29:Z31" si="38">IF(ISBLANK(A29),"",Y29&amp;"}"&amp;IF(OR(Z30="]",Z30="",ISBLANK(Z30)),"",","))</f>
+        <v>{"user":"emploji","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true},</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="M30" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="26"/>
+        <v>{"user":"emploji"</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="27"/>
+        <v>{"user":"emploji","typ":"Ferien"</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="28"/>
+        <v>{"user":"emploji","typ":"Ferien","text":""</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="29"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="30"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="31"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="32"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="33"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="V30" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="34"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="W30" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="35"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="X30" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="36"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Y30" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="37"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Z30" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="38"/>
+        <v>{"user":"emploji","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false},</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31">
+        <v>14</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="M31" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="26"/>
+        <v>{"user":"emploji"</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="27"/>
+        <v>{"user":"emploji","typ":"Krankheit"</v>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="28"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":""</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="29"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02"</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="30"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19"</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="31"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="32"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="33"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="V31" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="34"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="35"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="X31" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="36"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Y31" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="37"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false</v>
       </c>
       <c r="Z31" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="38"/>
+        <v>{"user":"emploji","typ":"Krankheit","text":"","fromDate":"2017-05-02","toDate":"2017-05-19","days":14,"commit":false},</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M32" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel"</v>
       </c>
       <c r="P32" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":""</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R32" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T32" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="V32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="W32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="X32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Y32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
       </c>
       <c r="Z32" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true}</v>
       </c>
     </row>
     <row r="33" spans="13:26" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
optimize LUIs.ai, add missing icons, add test data for "User", add "Gratistip" before intent
</commit_message>
<xml_diff>
--- a/import/datastore/Absences.xlsx
+++ b/import/datastore/Absences.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="73">
   <si>
     <t>ski</t>
   </si>
@@ -147,9 +147,6 @@
     <t>[</t>
   </si>
   <si>
-    <t>]</t>
-  </si>
-  <si>
     <t>Tabellen Konvertierung EXCEL -&gt; JSON</t>
   </si>
   <si>
@@ -229,6 +226,30 @@
   </si>
   <si>
     <t>Wohnungswechsel</t>
+  </si>
+  <si>
+    <t>Unfall</t>
+  </si>
+  <si>
+    <t>Heirat</t>
+  </si>
+  <si>
+    <t>Jubiläum</t>
+  </si>
+  <si>
+    <t>Mutterschaftsurlaub</t>
+  </si>
+  <si>
+    <t>Militär+Zivilschutz</t>
+  </si>
+  <si>
+    <t>Unbezahlt</t>
+  </si>
+  <si>
+    <t>Todesfall</t>
+  </si>
+  <si>
+    <t>Kompensation</t>
   </si>
 </sst>
 </file>
@@ -3091,10 +3112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z56"/>
+  <dimension ref="A1:Z57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z57" sqref="Z4:Z57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3107,15 +3128,15 @@
   <sheetData>
     <row r="1" spans="1:26" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -3220,7 +3241,7 @@
         <v>36</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -3280,22 +3301,22 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M5" t="str">
         <f>"{"</f>
@@ -3356,25 +3377,25 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" ref="M6:M55" si="3">"{"</f>
+        <f t="shared" ref="M6:M57" si="3">"{"</f>
         <v>{</v>
       </c>
       <c r="N6" t="str">
@@ -3432,22 +3453,22 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F7">
         <v>14</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="3"/>
@@ -3508,22 +3529,22 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="3"/>
@@ -3584,22 +3605,22 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="3"/>
@@ -3660,22 +3681,22 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F10">
         <v>14</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="3"/>
@@ -3736,22 +3757,22 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="3"/>
@@ -3812,22 +3833,22 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12">
         <v>5</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="3"/>
@@ -3888,22 +3909,22 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F13">
         <v>14</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="3"/>
@@ -3964,22 +3985,22 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="F14">
         <v>19</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="3"/>
@@ -4040,22 +4061,22 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F15">
         <v>5</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="3"/>
@@ -4116,22 +4137,22 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F16">
         <v>5</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="3"/>
@@ -4192,22 +4213,22 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F17">
         <v>3</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="3"/>
@@ -4268,22 +4289,22 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18">
         <v>5</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="3"/>
@@ -4344,22 +4365,22 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F19">
         <v>14</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="3"/>
@@ -4420,22 +4441,22 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F20">
         <v>3</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="3"/>
@@ -4496,22 +4517,22 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21">
         <v>5</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="3"/>
@@ -4572,22 +4593,22 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
         <v>31</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F22">
         <v>14</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="3"/>
@@ -4648,22 +4669,22 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F23">
         <v>3</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="3"/>
@@ -4724,22 +4745,22 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24">
         <v>5</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="3"/>
@@ -4800,22 +4821,22 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F25">
         <v>14</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="3"/>
@@ -4876,22 +4897,22 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F26">
         <v>3</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="3"/>
@@ -4952,22 +4973,22 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27">
         <v>5</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="3"/>
@@ -5028,22 +5049,22 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F28">
         <v>14</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="3"/>
@@ -5104,22 +5125,22 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F29">
         <v>3</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="3"/>
@@ -5180,22 +5201,22 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30">
         <v>5</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="3"/>
@@ -5256,22 +5277,22 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F31">
         <v>14</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="3"/>
@@ -5332,16 +5353,16 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F32">
         <v>3</v>
@@ -5379,1370 +5400,1931 @@
       </c>
       <c r="T32" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y32" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z32" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":true}</v>
+        <v>{"user":"lorenz-haenggi","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="33" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M33" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" ref="N33" si="39">IF(N$4=0,M33,M33&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A33&amp;"""",IF(N$3=2,IF(A33=1,"true", "false"),A33))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" ref="O33" si="40">IF(O$4=0,N33,N33&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B33&amp;"""",IF(O$3=2,IF(B33=1,"true", "false"),B33))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs"</v>
       </c>
       <c r="P33" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" ref="P33" si="41">IF(P$4=0,O33,O33&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C33&amp;"""",IF(P$3=2,IF(C33=1,"true", "false"),C33))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":""</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" ref="Q33" si="42">IF(Q$4=0,P33,P33&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D33&amp;"""",IF(Q$3=2,IF(D33=1,"true", "false"),D33))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" ref="R33" si="43">IF(R$4=0,Q33,Q33&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E33&amp;"""",IF(R$3=2,IF(E33=1,"true", "false"),E33))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" ref="S33" si="44">IF(S$4=0,R33,R33&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F33&amp;"""",IF(S$3=2,IF(F33=1,"true", "false"),F33))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="T33" si="45">IF(T$4=0,S33,S33&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G33&amp;"""",IF(T$3=2,IF(G33=1,"true", "false"),G33))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U33" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="U33" si="46">IF(U$4=0,T33,T33&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H33&amp;"""",IF(U$3=2,IF(H33=1,"true", "false"),H33))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V33" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="V33" si="47">IF(V$4=0,U33,U33&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I33&amp;"""",IF(V$3=2,IF(I33=1,"true", "false"),I33))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W33" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="W33" si="48">IF(W$4=0,V33,V33&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J33&amp;"""",IF(W$3=2,IF(J33=1,"true", "false"),J33))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X33" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="X33" si="49">IF(X$4=0,W33,W33&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K33&amp;"""",IF(X$3=2,IF(K33=1,"true", "false"),K33))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="Y33" si="50">IF(Y$4=0,X33,X33&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L33&amp;"""",IF(Y$3=2,IF(L33=1,"true", "false"),L33))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z33" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" ref="Z33" si="51">IF(ISBLANK(A33),"",Y33&amp;"}"&amp;IF(OR(Z34="]",Z34="",ISBLANK(Z34)),"",","))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="34" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M34" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" ref="N34:N40" si="52">IF(N$4=0,M34,M34&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A34&amp;"""",IF(N$3=2,IF(A34=1,"true", "false"),A34))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" ref="O34:O40" si="53">IF(O$4=0,N34,N34&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B34&amp;"""",IF(O$3=2,IF(B34=1,"true", "false"),B34))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall"</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" ref="P34:P40" si="54">IF(P$4=0,O34,O34&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C34&amp;"""",IF(P$3=2,IF(C34=1,"true", "false"),C34))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":""</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" ref="Q34:Q40" si="55">IF(Q$4=0,P34,P34&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D34&amp;"""",IF(Q$3=2,IF(D34=1,"true", "false"),D34))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" ref="R34:R40" si="56">IF(R$4=0,Q34,Q34&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E34&amp;"""",IF(R$3=2,IF(E34=1,"true", "false"),E34))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" ref="S34:S40" si="57">IF(S$4=0,R34,R34&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F34&amp;"""",IF(S$3=2,IF(F34=1,"true", "false"),F34))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="T34:T40" si="58">IF(T$4=0,S34,S34&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G34&amp;"""",IF(T$3=2,IF(G34=1,"true", "false"),G34))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U34" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="U34:U40" si="59">IF(U$4=0,T34,T34&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H34&amp;"""",IF(U$3=2,IF(H34=1,"true", "false"),H34))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V34" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="V34:V40" si="60">IF(V$4=0,U34,U34&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I34&amp;"""",IF(V$3=2,IF(I34=1,"true", "false"),I34))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W34" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="W34:W40" si="61">IF(W$4=0,V34,V34&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J34&amp;"""",IF(W$3=2,IF(J34=1,"true", "false"),J34))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X34" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="X34:X40" si="62">IF(X$4=0,W34,W34&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K34&amp;"""",IF(X$3=2,IF(K34=1,"true", "false"),K34))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="Y34:Y40" si="63">IF(Y$4=0,X34,X34&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L34&amp;"""",IF(Y$3=2,IF(L34=1,"true", "false"),L34))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z34" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" ref="Z34:Z40" si="64">IF(ISBLANK(A34),"",Y34&amp;"}"&amp;IF(OR(Z35="]",Z35="",ISBLANK(Z35)),"",","))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="35" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M35" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O35" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien"</v>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":""</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R35" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="56"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="57"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="58"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U35" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="59"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V35" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="60"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W35" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="61"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X35" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="62"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="63"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z35" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="64"/>
+        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="36" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M36" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O36" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit"</v>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":""</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R36" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="56"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="57"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="58"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="59"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V36" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="60"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W36" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="61"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X36" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="62"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y36" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="63"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z36" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="64"/>
+        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="37" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M37" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O37" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat"</v>
       </c>
       <c r="P37" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":""</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R37" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="56"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="57"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="58"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="59"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V37" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="60"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W37" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="61"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X37" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="62"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y37" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="63"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z37" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="64"/>
+        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="38" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M38" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O38" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum"</v>
       </c>
       <c r="P38" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":""</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="56"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="57"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="58"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="59"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V38" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="60"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W38" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="61"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X38" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="62"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y38" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="63"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z38" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="64"/>
+        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="39" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M39" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O39" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub"</v>
       </c>
       <c r="P39" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":""</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="56"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="57"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="58"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U39" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="59"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V39" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="60"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W39" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="61"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X39" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="62"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y39" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="63"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z39" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="64"/>
+        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="40" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M40" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N40" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O40" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz"</v>
       </c>
       <c r="P40" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":""</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="56"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S40" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="57"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="58"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U40" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="59"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V40" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="60"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W40" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="61"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X40" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="62"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y40" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="63"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z40" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="64"/>
+        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="41" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M41" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N41" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" ref="N41:N42" si="65">IF(N$4=0,M41,M41&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A41&amp;"""",IF(N$3=2,IF(A41=1,"true", "false"),A41))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O41" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" ref="O41:O42" si="66">IF(O$4=0,N41,N41&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B41&amp;"""",IF(O$3=2,IF(B41=1,"true", "false"),B41))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt"</v>
       </c>
       <c r="P41" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" ref="P41:P42" si="67">IF(P$4=0,O41,O41&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C41&amp;"""",IF(P$3=2,IF(C41=1,"true", "false"),C41))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":""</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" ref="Q41:Q42" si="68">IF(Q$4=0,P41,P41&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D41&amp;"""",IF(Q$3=2,IF(D41=1,"true", "false"),D41))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" ref="R41:R42" si="69">IF(R$4=0,Q41,Q41&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E41&amp;"""",IF(R$3=2,IF(E41=1,"true", "false"),E41))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S41" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" ref="S41:S42" si="70">IF(S$4=0,R41,R41&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F41&amp;"""",IF(S$3=2,IF(F41=1,"true", "false"),F41))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="T41:T42" si="71">IF(T$4=0,S41,S41&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G41&amp;"""",IF(T$3=2,IF(G41=1,"true", "false"),G41))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U41" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="U41:U42" si="72">IF(U$4=0,T41,T41&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H41&amp;"""",IF(U$3=2,IF(H41=1,"true", "false"),H41))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V41" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="V41:V42" si="73">IF(V$4=0,U41,U41&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I41&amp;"""",IF(V$3=2,IF(I41=1,"true", "false"),I41))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W41" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="W41:W42" si="74">IF(W$4=0,V41,V41&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J41&amp;"""",IF(W$3=2,IF(J41=1,"true", "false"),J41))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X41" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="X41:X42" si="75">IF(X$4=0,W41,W41&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K41&amp;"""",IF(X$3=2,IF(K41=1,"true", "false"),K41))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y41" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="Y41:Y42" si="76">IF(Y$4=0,X41,X41&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L41&amp;"""",IF(Y$3=2,IF(L41=1,"true", "false"),L41))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z41" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" ref="Z41:Z42" si="77">IF(ISBLANK(A41),"",Y41&amp;"}"&amp;IF(OR(Z42="]",Z42="",ISBLANK(Z42)),"",","))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="42" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M42" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N42" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="65"/>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O42" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="66"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub"</v>
       </c>
       <c r="P42" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="67"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":""</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="68"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="69"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="70"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="71"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="72"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V42" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="73"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W42" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="74"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X42" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="75"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="76"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z42" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="77"/>
+        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="43" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M43" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N43" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" ref="N43" si="78">IF(N$4=0,M43,M43&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A43&amp;"""",IF(N$3=2,IF(A43=1,"true", "false"),A43))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O43" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" ref="O43" si="79">IF(O$4=0,N43,N43&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B43&amp;"""",IF(O$3=2,IF(B43=1,"true", "false"),B43))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall"</v>
       </c>
       <c r="P43" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" ref="P43" si="80">IF(P$4=0,O43,O43&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C43&amp;"""",IF(P$3=2,IF(C43=1,"true", "false"),C43))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":""</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" ref="Q43" si="81">IF(Q$4=0,P43,P43&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D43&amp;"""",IF(Q$3=2,IF(D43=1,"true", "false"),D43))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" ref="R43" si="82">IF(R$4=0,Q43,Q43&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E43&amp;"""",IF(R$3=2,IF(E43=1,"true", "false"),E43))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S43" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" ref="S43" si="83">IF(S$4=0,R43,R43&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F43&amp;"""",IF(S$3=2,IF(F43=1,"true", "false"),F43))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="T43" si="84">IF(T$4=0,S43,S43&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G43&amp;"""",IF(T$3=2,IF(G43=1,"true", "false"),G43))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U43" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="U43" si="85">IF(U$4=0,T43,T43&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H43&amp;"""",IF(U$3=2,IF(H43=1,"true", "false"),H43))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V43" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="V43" si="86">IF(V$4=0,U43,U43&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I43&amp;"""",IF(V$3=2,IF(I43=1,"true", "false"),I43))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W43" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="W43" si="87">IF(W$4=0,V43,V43&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J43&amp;"""",IF(W$3=2,IF(J43=1,"true", "false"),J43))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X43" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="X43" si="88">IF(X$4=0,W43,W43&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K43&amp;"""",IF(X$3=2,IF(K43=1,"true", "false"),K43))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y43" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="Y43" si="89">IF(Y$4=0,X43,X43&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L43&amp;"""",IF(Y$3=2,IF(L43=1,"true", "false"),L43))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z43" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" ref="Z43" si="90">IF(ISBLANK(A43),"",Y43&amp;"}"&amp;IF(OR(Z44="]",Z44="",ISBLANK(Z44)),"",","))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="44" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M44" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N44" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" ref="N44:N56" si="91">IF(N$4=0,M44,M44&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A44&amp;"""",IF(N$3=2,IF(A44=1,"true", "false"),A44))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="O44" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" ref="O44:O56" si="92">IF(O$4=0,N44,N44&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B44&amp;"""",IF(O$3=2,IF(B44=1,"true", "false"),B44))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation"</v>
       </c>
       <c r="P44" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" ref="P44:P56" si="93">IF(P$4=0,O44,O44&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C44&amp;"""",IF(P$3=2,IF(C44=1,"true", "false"),C44))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":""</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" ref="Q44:Q56" si="94">IF(Q$4=0,P44,P44&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D44&amp;"""",IF(Q$3=2,IF(D44=1,"true", "false"),D44))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" ref="R44:R56" si="95">IF(R$4=0,Q44,Q44&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E44&amp;"""",IF(R$3=2,IF(E44=1,"true", "false"),E44))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S44" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" ref="S44:S56" si="96">IF(S$4=0,R44,R44&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F44&amp;"""",IF(S$3=2,IF(F44=1,"true", "false"),F44))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="T44:T56" si="97">IF(T$4=0,S44,S44&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G44&amp;"""",IF(T$3=2,IF(G44=1,"true", "false"),G44))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U44" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="U44:U56" si="98">IF(U$4=0,T44,T44&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H44&amp;"""",IF(U$3=2,IF(H44=1,"true", "false"),H44))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V44" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="V44:V56" si="99">IF(V$4=0,U44,U44&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I44&amp;"""",IF(V$3=2,IF(I44=1,"true", "false"),I44))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W44" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="W44:W56" si="100">IF(W$4=0,V44,V44&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J44&amp;"""",IF(W$3=2,IF(J44=1,"true", "false"),J44))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X44" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="X44:X56" si="101">IF(X$4=0,W44,W44&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K44&amp;"""",IF(X$3=2,IF(K44=1,"true", "false"),K44))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y44" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" ref="Y44:Y56" si="102">IF(Y$4=0,X44,X44&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L44&amp;"""",IF(Y$3=2,IF(L44=1,"true", "false"),L44))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z44" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" ref="Z44:Z56" si="103">IF(ISBLANK(A44),"",Y44&amp;"}"&amp;IF(OR(Z45="]",Z45="",ISBLANK(Z45)),"",","))</f>
+        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="45" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M45" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N45" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O45" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Wohnungswechsel"</v>
       </c>
       <c r="P45" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":""</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S45" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U45" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V45" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W45" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X45" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y45" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z45" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="46" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M46" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N46" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O46" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Kurs"</v>
       </c>
       <c r="P46" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Kurs","text":""</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U46" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V46" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W46" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X46" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z46" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="47" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M47" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N47" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O47" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Unfall"</v>
       </c>
       <c r="P47" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Unfall","text":""</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R47" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S47" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U47" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V47" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W47" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X47" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y47" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z47" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="48" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M48" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N48" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O48" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Ferien"</v>
       </c>
       <c r="P48" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Ferien","text":""</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R48" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S48" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U48" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V48" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W48" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X48" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y48" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z48" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="49" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M49" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N49" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O49" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Krankheit"</v>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Krankheit","text":""</v>
       </c>
       <c r="Q49" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R49" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S49" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U49" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V49" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W49" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X49" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y49" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z49" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="50" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M50" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N50" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O50" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Heirat"</v>
       </c>
       <c r="P50" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Heirat","text":""</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S50" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U50" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V50" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W50" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X50" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y50" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z50" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="51" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M51" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N51" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O51" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Jubiläum"</v>
       </c>
       <c r="P51" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Jubiläum","text":""</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S51" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U51" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V51" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W51" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X51" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y51" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z51" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="52" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M52" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N52" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O52" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub"</v>
       </c>
       <c r="P52" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":""</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R52" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S52" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T52" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U52" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V52" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W52" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X52" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y52" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z52" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="53" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M53" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N53" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O53" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz"</v>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":""</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R53" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S53" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U53" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V53" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W53" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X53" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y53" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z53" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="54" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M54" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O54" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Unbezahlt"</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":""</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R54" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S54" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U54" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V54" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W54" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X54" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y54" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z54" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="55" spans="13:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="M55" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N55" t="str">
-        <f t="shared" si="4"/>
-        <v>{"user":""</v>
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O55" t="str">
-        <f t="shared" si="5"/>
-        <v>{"user":"","typ":""</v>
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub"</v>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="6"/>
-        <v>{"user":"","typ":"","text":""</v>
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":""</v>
       </c>
       <c r="Q55" t="str">
-        <f t="shared" si="7"/>
-        <v>{"user":"","typ":"","text":"","fromDate":""</v>
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R55" t="str">
-        <f t="shared" si="8"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S55" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T55" t="str">
-        <f t="shared" si="10"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U55" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V55" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W55" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X55" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y55" t="str">
-        <f t="shared" si="11"/>
-        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z55" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
-    <row r="56" spans="13:26" x14ac:dyDescent="0.2">
-      <c r="Z56" s="5" t="s">
-        <v>38</v>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="3"/>
+        <v>{</v>
+      </c>
+      <c r="N56" t="str">
+        <f t="shared" si="91"/>
+        <v>{"user":"User"</v>
+      </c>
+      <c r="O56" t="str">
+        <f t="shared" si="92"/>
+        <v>{"user":"User","typ":"Todesfall"</v>
+      </c>
+      <c r="P56" t="str">
+        <f t="shared" si="93"/>
+        <v>{"user":"User","typ":"Todesfall","text":""</v>
+      </c>
+      <c r="Q56" t="str">
+        <f t="shared" si="94"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15"</v>
+      </c>
+      <c r="R56" t="str">
+        <f t="shared" si="95"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+      </c>
+      <c r="S56" t="str">
+        <f t="shared" si="96"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+      </c>
+      <c r="T56" t="str">
+        <f t="shared" si="97"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="U56" t="str">
+        <f t="shared" si="98"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="V56" t="str">
+        <f t="shared" si="99"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="W56" t="str">
+        <f t="shared" si="100"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="X56" t="str">
+        <f t="shared" si="101"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="Y56" t="str">
+        <f t="shared" si="102"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="Z56" t="str">
+        <f t="shared" si="103"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M57" t="str">
+        <f t="shared" si="3"/>
+        <v>{</v>
+      </c>
+      <c r="N57" t="str">
+        <f t="shared" ref="N57" si="104">IF(N$4=0,M57,M57&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A57&amp;"""",IF(N$3=2,IF(A57=1,"true", "false"),A57))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":"User"</v>
+      </c>
+      <c r="O57" t="str">
+        <f t="shared" ref="O57" si="105">IF(O$4=0,N57,N57&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B57&amp;"""",IF(O$3=2,IF(B57=1,"true", "false"),B57))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation"</v>
+      </c>
+      <c r="P57" t="str">
+        <f t="shared" ref="P57" si="106">IF(P$4=0,O57,O57&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C57&amp;"""",IF(P$3=2,IF(C57=1,"true", "false"),C57))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":""</v>
+      </c>
+      <c r="Q57" t="str">
+        <f t="shared" ref="Q57" si="107">IF(Q$4=0,P57,P57&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D57&amp;"""",IF(Q$3=2,IF(D57=1,"true", "false"),D57))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15"</v>
+      </c>
+      <c r="R57" t="str">
+        <f t="shared" ref="R57" si="108">IF(R$4=0,Q57,Q57&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E57&amp;"""",IF(R$3=2,IF(E57=1,"true", "false"),E57))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+      </c>
+      <c r="S57" t="str">
+        <f t="shared" ref="S57" si="109">IF(S$4=0,R57,R57&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F57&amp;"""",IF(S$3=2,IF(F57=1,"true", "false"),F57))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+      </c>
+      <c r="T57" t="str">
+        <f t="shared" ref="T57" si="110">IF(T$4=0,S57,S57&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G57&amp;"""",IF(T$3=2,IF(G57=1,"true", "false"),G57))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="U57" t="str">
+        <f t="shared" ref="U57" si="111">IF(U$4=0,T57,T57&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H57&amp;"""",IF(U$3=2,IF(H57=1,"true", "false"),H57))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="V57" t="str">
+        <f t="shared" ref="V57" si="112">IF(V$4=0,U57,U57&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I57&amp;"""",IF(V$3=2,IF(I57=1,"true", "false"),I57))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="W57" t="str">
+        <f t="shared" ref="W57" si="113">IF(W$4=0,V57,V57&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J57&amp;"""",IF(W$3=2,IF(J57=1,"true", "false"),J57))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="X57" t="str">
+        <f t="shared" ref="X57" si="114">IF(X$4=0,W57,W57&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K57&amp;"""",IF(X$3=2,IF(K57=1,"true", "false"),K57))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="Y57" t="str">
+        <f t="shared" ref="Y57" si="115">IF(Y$4=0,X57,X57&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L57&amp;"""",IF(Y$3=2,IF(L57=1,"true", "false"),L57))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+      </c>
+      <c r="Z57" t="str">
+        <f t="shared" ref="Z57" si="116">IF(ISBLANK(A57),"",Y57&amp;"}"&amp;IF(OR(Z58="]",Z58="",ISBLANK(Z58)),"",","))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove test-data for Lolo for demo
</commit_message>
<xml_diff>
--- a/import/datastore/Absences.xlsx
+++ b/import/datastore/Absences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="73">
   <si>
     <t>ski</t>
   </si>
@@ -593,7 +593,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -648,7 +648,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -703,7 +703,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -760,7 +760,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -817,7 +817,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -874,7 +874,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -929,7 +929,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -986,7 +986,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1041,7 +1041,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1098,7 +1098,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1155,7 +1155,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1212,7 +1212,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1267,7 +1267,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1324,7 +1324,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1379,7 +1379,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1434,7 +1434,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1489,7 +1489,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1546,7 +1546,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1601,7 +1601,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1656,7 +1656,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1713,7 +1713,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1768,7 +1768,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1823,7 +1823,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1880,7 +1880,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1937,7 +1937,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1994,7 +1994,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2049,7 +2049,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2106,7 +2106,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2161,7 +2161,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2216,7 +2216,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2271,7 +2271,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2328,7 +2328,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2383,7 +2383,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2438,7 +2438,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2495,7 +2495,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2550,7 +2550,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2605,7 +2605,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2662,7 +2662,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2719,7 +2719,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2776,7 +2776,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3115,7 +3115,7 @@
   <dimension ref="A1:Z57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z57" sqref="Z4:Z57"/>
+      <selection activeCell="Z45" sqref="Z4:Z45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3399,35 +3399,35 @@
         <v>{</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" ref="N6:N55" si="4">IF(N$4=0,M6,M6&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A6&amp;"""",IF(N$3=2,IF(A6=1,"true", "false"),A6))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <f t="shared" ref="N6:N45" si="4">IF(N$4=0,M6,M6&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A6&amp;"""",IF(N$3=2,IF(A6=1,"true", "false"),A6))&amp;IF(ISBLANK(O$3),"},",""))</f>
         <v>{"user":"brm"</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" ref="O6:O55" si="5">IF(O$4=0,N6,N6&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B6&amp;"""",IF(O$3=2,IF(B6=1,"true", "false"),B6))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <f t="shared" ref="O6:O45" si="5">IF(O$4=0,N6,N6&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B6&amp;"""",IF(O$3=2,IF(B6=1,"true", "false"),B6))&amp;IF(ISBLANK(P$3),"},",""))</f>
         <v>{"user":"brm","typ":"Ferien"</v>
       </c>
       <c r="P6" t="str">
-        <f t="shared" ref="P6:P55" si="6">IF(P$4=0,O6,O6&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C6&amp;"""",IF(P$3=2,IF(C6=1,"true", "false"),C6))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" ref="P6:P45" si="6">IF(P$4=0,O6,O6&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C6&amp;"""",IF(P$3=2,IF(C6=1,"true", "false"),C6))&amp;IF(ISBLANK(Q$3),"},",""))</f>
         <v>{"user":"brm","typ":"Ferien","text":""</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" ref="Q6:Q55" si="7">IF(Q$4=0,P6,P6&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D6&amp;"""",IF(Q$3=2,IF(D6=1,"true", "false"),D6))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q6:Q45" si="7">IF(Q$4=0,P6,P6&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D6&amp;"""",IF(Q$3=2,IF(D6=1,"true", "false"),D6))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15"</v>
       </c>
       <c r="R6" t="str">
-        <f t="shared" ref="R6:R55" si="8">IF(R$4=0,Q6,Q6&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E6&amp;"""",IF(R$3=2,IF(E6=1,"true", "false"),E6))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <f t="shared" ref="R6:R45" si="8">IF(R$4=0,Q6,Q6&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E6&amp;"""",IF(R$3=2,IF(E6=1,"true", "false"),E6))&amp;IF(ISBLANK(S$3),"},",""))</f>
         <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22"</v>
       </c>
       <c r="S6" t="str">
-        <f t="shared" ref="S6:S55" si="9">IF(S$4=0,R6,R6&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F6&amp;"""",IF(S$3=2,IF(F6=1,"true", "false"),F6))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <f t="shared" ref="S6:S45" si="9">IF(S$4=0,R6,R6&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F6&amp;"""",IF(S$3=2,IF(F6=1,"true", "false"),F6))&amp;IF(ISBLANK(T$3),"},",""))</f>
         <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5</v>
       </c>
       <c r="T6" t="str">
-        <f t="shared" ref="T6:T55" si="10">IF(T$4=0,S6,S6&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G6&amp;"""",IF(T$3=2,IF(G6=1,"true", "false"),G6))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <f t="shared" ref="T6:T45" si="10">IF(T$4=0,S6,S6&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G6&amp;"""",IF(T$3=2,IF(G6=1,"true", "false"),G6))&amp;IF(ISBLANK(U$3),"},",""))</f>
         <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="U6" t="str">
-        <f t="shared" ref="U6:Y55" si="11">IF(U$4=0,T6,T6&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H6&amp;"""",IF(U$3=2,IF(H6=1,"true", "false"),H6))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <f t="shared" ref="U6:Y32" si="11">IF(U$4=0,T6,T6&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H6&amp;"""",IF(U$3=2,IF(H6=1,"true", "false"),H6))&amp;IF(ISBLANK(V$3),"},",""))</f>
         <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="V6" t="str">
@@ -3447,7 +3447,7 @@
         <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false</v>
       </c>
       <c r="Z6" t="str">
-        <f t="shared" ref="Z6:Z55" si="12">IF(ISBLANK(A6),"",Y6&amp;"}"&amp;IF(OR(Z7="]",Z7="",ISBLANK(Z7)),"",","))</f>
+        <f t="shared" ref="Z6:Z44" si="12">IF(ISBLANK(A6),"",Y6&amp;"}"&amp;IF(OR(Z7="]",Z7="",ISBLANK(Z7)),"",","))</f>
         <v>{"user":"brm","typ":"Ferien","text":"","fromDate":"2017-03-15","toDate":"2017-03-22","days":5,"commit":false},</v>
       </c>
     </row>
@@ -5429,10 +5429,10 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>49</v>
@@ -5451,64 +5451,64 @@
         <v>{</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" ref="N33" si="39">IF(N$4=0,M33,M33&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A33&amp;"""",IF(N$3=2,IF(A33=1,"true", "false"),A33))&amp;IF(ISBLANK(O$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" ref="O33" si="40">IF(O$4=0,N33,N33&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B33&amp;"""",IF(O$3=2,IF(B33=1,"true", "false"),B33))&amp;IF(ISBLANK(P$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Wohnungswechsel"</v>
       </c>
       <c r="P33" t="str">
-        <f t="shared" ref="P33" si="41">IF(P$4=0,O33,O33&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C33&amp;"""",IF(P$3=2,IF(C33=1,"true", "false"),C33))&amp;IF(ISBLANK(Q$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":""</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" ref="Q33" si="42">IF(Q$4=0,P33,P33&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D33&amp;"""",IF(Q$3=2,IF(D33=1,"true", "false"),D33))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" ref="R33" si="43">IF(R$4=0,Q33,Q33&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E33&amp;"""",IF(R$3=2,IF(E33=1,"true", "false"),E33))&amp;IF(ISBLANK(S$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" ref="S33" si="44">IF(S$4=0,R33,R33&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F33&amp;"""",IF(S$3=2,IF(F33=1,"true", "false"),F33))&amp;IF(ISBLANK(T$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" ref="T33" si="45">IF(T$4=0,S33,S33&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G33&amp;"""",IF(T$3=2,IF(G33=1,"true", "false"),G33))&amp;IF(ISBLANK(U$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U33" t="str">
-        <f t="shared" ref="U33" si="46">IF(U$4=0,T33,T33&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H33&amp;"""",IF(U$3=2,IF(H33=1,"true", "false"),H33))&amp;IF(ISBLANK(V$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="U33:U45" si="39">IF(U$4=0,T33,T33&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H33&amp;"""",IF(U$3=2,IF(H33=1,"true", "false"),H33))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V33" t="str">
-        <f t="shared" ref="V33" si="47">IF(V$4=0,U33,U33&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I33&amp;"""",IF(V$3=2,IF(I33=1,"true", "false"),I33))&amp;IF(ISBLANK(W$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="V33:V45" si="40">IF(V$4=0,U33,U33&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I33&amp;"""",IF(V$3=2,IF(I33=1,"true", "false"),I33))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W33" t="str">
-        <f t="shared" ref="W33" si="48">IF(W$4=0,V33,V33&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J33&amp;"""",IF(W$3=2,IF(J33=1,"true", "false"),J33))&amp;IF(ISBLANK(X$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="W33:W45" si="41">IF(W$4=0,V33,V33&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J33&amp;"""",IF(W$3=2,IF(J33=1,"true", "false"),J33))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X33" t="str">
-        <f t="shared" ref="X33" si="49">IF(X$4=0,W33,W33&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K33&amp;"""",IF(X$3=2,IF(K33=1,"true", "false"),K33))&amp;IF(ISBLANK(Y$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="X33:X45" si="42">IF(X$4=0,W33,W33&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K33&amp;"""",IF(X$3=2,IF(K33=1,"true", "false"),K33))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" ref="Y33" si="50">IF(Y$4=0,X33,X33&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L33&amp;"""",IF(Y$3=2,IF(L33=1,"true", "false"),L33))&amp;IF(ISBLANK(Z$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="Y33:Y45" si="43">IF(Y$4=0,X33,X33&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L33&amp;"""",IF(Y$3=2,IF(L33=1,"true", "false"),L33))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z33" t="str">
-        <f t="shared" ref="Z33" si="51">IF(ISBLANK(A33),"",Y33&amp;"}"&amp;IF(OR(Z34="]",Z34="",ISBLANK(Z34)),"",","))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>49</v>
@@ -5527,64 +5527,64 @@
         <v>{</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" ref="N34:N40" si="52">IF(N$4=0,M34,M34&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A34&amp;"""",IF(N$3=2,IF(A34=1,"true", "false"),A34))&amp;IF(ISBLANK(O$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" ref="O34:O40" si="53">IF(O$4=0,N34,N34&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B34&amp;"""",IF(O$3=2,IF(B34=1,"true", "false"),B34))&amp;IF(ISBLANK(P$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Kurs"</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" ref="P34:P40" si="54">IF(P$4=0,O34,O34&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C34&amp;"""",IF(P$3=2,IF(C34=1,"true", "false"),C34))&amp;IF(ISBLANK(Q$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Kurs","text":""</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" ref="Q34:Q40" si="55">IF(Q$4=0,P34,P34&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D34&amp;"""",IF(Q$3=2,IF(D34=1,"true", "false"),D34))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" ref="R34:R40" si="56">IF(R$4=0,Q34,Q34&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E34&amp;"""",IF(R$3=2,IF(E34=1,"true", "false"),E34))&amp;IF(ISBLANK(S$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" ref="S34:S40" si="57">IF(S$4=0,R34,R34&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F34&amp;"""",IF(S$3=2,IF(F34=1,"true", "false"),F34))&amp;IF(ISBLANK(T$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" ref="T34:T40" si="58">IF(T$4=0,S34,S34&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G34&amp;"""",IF(T$3=2,IF(G34=1,"true", "false"),G34))&amp;IF(ISBLANK(U$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U34" t="str">
-        <f t="shared" ref="U34:U40" si="59">IF(U$4=0,T34,T34&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H34&amp;"""",IF(U$3=2,IF(H34=1,"true", "false"),H34))&amp;IF(ISBLANK(V$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V34" t="str">
-        <f t="shared" ref="V34:V40" si="60">IF(V$4=0,U34,U34&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I34&amp;"""",IF(V$3=2,IF(I34=1,"true", "false"),I34))&amp;IF(ISBLANK(W$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W34" t="str">
-        <f t="shared" ref="W34:W40" si="61">IF(W$4=0,V34,V34&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J34&amp;"""",IF(W$3=2,IF(J34=1,"true", "false"),J34))&amp;IF(ISBLANK(X$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X34" t="str">
-        <f t="shared" ref="X34:X40" si="62">IF(X$4=0,W34,W34&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K34&amp;"""",IF(X$3=2,IF(K34=1,"true", "false"),K34))&amp;IF(ISBLANK(Y$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" ref="Y34:Y40" si="63">IF(Y$4=0,X34,X34&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L34&amp;"""",IF(Y$3=2,IF(L34=1,"true", "false"),L34))&amp;IF(ISBLANK(Z$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z34" t="str">
-        <f t="shared" ref="Z34:Z40" si="64">IF(ISBLANK(A34),"",Y34&amp;"}"&amp;IF(OR(Z35="]",Z35="",ISBLANK(Z35)),"",","))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>49</v>
@@ -5603,64 +5603,64 @@
         <v>{</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="52"/>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O35" t="str">
-        <f t="shared" si="53"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Unfall"</v>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="54"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Unfall","text":""</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="55"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R35" t="str">
-        <f t="shared" si="56"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="57"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="58"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U35" t="str">
-        <f t="shared" si="59"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V35" t="str">
-        <f t="shared" si="60"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W35" t="str">
-        <f t="shared" si="61"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X35" t="str">
-        <f t="shared" si="62"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="63"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z35" t="str">
-        <f t="shared" si="64"/>
-        <v>{"user":"lorenz-haenggi","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>49</v>
@@ -5679,64 +5679,64 @@
         <v>{</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="52"/>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O36" t="str">
-        <f t="shared" si="53"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Ferien"</v>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="54"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Ferien","text":""</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="55"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R36" t="str">
-        <f t="shared" si="56"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="57"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="58"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="59"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V36" t="str">
-        <f t="shared" si="60"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W36" t="str">
-        <f t="shared" si="61"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X36" t="str">
-        <f t="shared" si="62"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y36" t="str">
-        <f t="shared" si="63"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z36" t="str">
-        <f t="shared" si="64"/>
-        <v>{"user":"lorenz-haenggi","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>49</v>
@@ -5755,64 +5755,64 @@
         <v>{</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="52"/>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O37" t="str">
-        <f t="shared" si="53"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Krankheit"</v>
       </c>
       <c r="P37" t="str">
-        <f t="shared" si="54"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Krankheit","text":""</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="55"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R37" t="str">
-        <f t="shared" si="56"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="57"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="58"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="59"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V37" t="str">
-        <f t="shared" si="60"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W37" t="str">
-        <f t="shared" si="61"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X37" t="str">
-        <f t="shared" si="62"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y37" t="str">
-        <f t="shared" si="63"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z37" t="str">
-        <f t="shared" si="64"/>
-        <v>{"user":"lorenz-haenggi","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>49</v>
@@ -5831,64 +5831,64 @@
         <v>{</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="52"/>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O38" t="str">
-        <f t="shared" si="53"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Heirat"</v>
       </c>
       <c r="P38" t="str">
-        <f t="shared" si="54"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Heirat","text":""</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="55"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" si="56"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="57"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="58"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="59"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V38" t="str">
-        <f t="shared" si="60"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W38" t="str">
-        <f t="shared" si="61"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X38" t="str">
-        <f t="shared" si="62"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y38" t="str">
-        <f t="shared" si="63"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z38" t="str">
-        <f t="shared" si="64"/>
-        <v>{"user":"lorenz-haenggi","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>49</v>
@@ -5907,64 +5907,64 @@
         <v>{</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="52"/>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O39" t="str">
-        <f t="shared" si="53"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Jubiläum"</v>
       </c>
       <c r="P39" t="str">
-        <f t="shared" si="54"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Jubiläum","text":""</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="55"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="56"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="57"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="58"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U39" t="str">
-        <f t="shared" si="59"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V39" t="str">
-        <f t="shared" si="60"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W39" t="str">
-        <f t="shared" si="61"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X39" t="str">
-        <f t="shared" si="62"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y39" t="str">
-        <f t="shared" si="63"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z39" t="str">
-        <f t="shared" si="64"/>
-        <v>{"user":"lorenz-haenggi","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>49</v>
@@ -5983,64 +5983,64 @@
         <v>{</v>
       </c>
       <c r="N40" t="str">
-        <f t="shared" si="52"/>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O40" t="str">
-        <f t="shared" si="53"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub"</v>
       </c>
       <c r="P40" t="str">
-        <f t="shared" si="54"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":""</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="55"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="56"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S40" t="str">
-        <f t="shared" si="57"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="58"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U40" t="str">
-        <f t="shared" si="59"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V40" t="str">
-        <f t="shared" si="60"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W40" t="str">
-        <f t="shared" si="61"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X40" t="str">
-        <f t="shared" si="62"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y40" t="str">
-        <f t="shared" si="63"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z40" t="str">
-        <f t="shared" si="64"/>
-        <v>{"user":"lorenz-haenggi","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>49</v>
@@ -6059,64 +6059,64 @@
         <v>{</v>
       </c>
       <c r="N41" t="str">
-        <f t="shared" ref="N41:N42" si="65">IF(N$4=0,M41,M41&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A41&amp;"""",IF(N$3=2,IF(A41=1,"true", "false"),A41))&amp;IF(ISBLANK(O$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O41" t="str">
-        <f t="shared" ref="O41:O42" si="66">IF(O$4=0,N41,N41&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B41&amp;"""",IF(O$3=2,IF(B41=1,"true", "false"),B41))&amp;IF(ISBLANK(P$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz"</v>
       </c>
       <c r="P41" t="str">
-        <f t="shared" ref="P41:P42" si="67">IF(P$4=0,O41,O41&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C41&amp;"""",IF(P$3=2,IF(C41=1,"true", "false"),C41))&amp;IF(ISBLANK(Q$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":""</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" ref="Q41:Q42" si="68">IF(Q$4=0,P41,P41&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D41&amp;"""",IF(Q$3=2,IF(D41=1,"true", "false"),D41))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" ref="R41:R42" si="69">IF(R$4=0,Q41,Q41&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E41&amp;"""",IF(R$3=2,IF(E41=1,"true", "false"),E41))&amp;IF(ISBLANK(S$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S41" t="str">
-        <f t="shared" ref="S41:S42" si="70">IF(S$4=0,R41,R41&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F41&amp;"""",IF(S$3=2,IF(F41=1,"true", "false"),F41))&amp;IF(ISBLANK(T$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" ref="T41:T42" si="71">IF(T$4=0,S41,S41&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G41&amp;"""",IF(T$3=2,IF(G41=1,"true", "false"),G41))&amp;IF(ISBLANK(U$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U41" t="str">
-        <f t="shared" ref="U41:U42" si="72">IF(U$4=0,T41,T41&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H41&amp;"""",IF(U$3=2,IF(H41=1,"true", "false"),H41))&amp;IF(ISBLANK(V$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V41" t="str">
-        <f t="shared" ref="V41:V42" si="73">IF(V$4=0,U41,U41&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I41&amp;"""",IF(V$3=2,IF(I41=1,"true", "false"),I41))&amp;IF(ISBLANK(W$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W41" t="str">
-        <f t="shared" ref="W41:W42" si="74">IF(W$4=0,V41,V41&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J41&amp;"""",IF(W$3=2,IF(J41=1,"true", "false"),J41))&amp;IF(ISBLANK(X$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X41" t="str">
-        <f t="shared" ref="X41:X42" si="75">IF(X$4=0,W41,W41&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K41&amp;"""",IF(X$3=2,IF(K41=1,"true", "false"),K41))&amp;IF(ISBLANK(Y$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y41" t="str">
-        <f t="shared" ref="Y41:Y42" si="76">IF(Y$4=0,X41,X41&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L41&amp;"""",IF(Y$3=2,IF(L41=1,"true", "false"),L41))&amp;IF(ISBLANK(Z$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z41" t="str">
-        <f t="shared" ref="Z41:Z42" si="77">IF(ISBLANK(A41),"",Y41&amp;"}"&amp;IF(OR(Z42="]",Z42="",ISBLANK(Z42)),"",","))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>49</v>
@@ -6135,64 +6135,64 @@
         <v>{</v>
       </c>
       <c r="N42" t="str">
-        <f t="shared" si="65"/>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O42" t="str">
-        <f t="shared" si="66"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Unbezahlt"</v>
       </c>
       <c r="P42" t="str">
-        <f t="shared" si="67"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":""</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="68"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="69"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="70"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="71"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="72"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V42" t="str">
-        <f t="shared" si="73"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W42" t="str">
-        <f t="shared" si="74"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X42" t="str">
-        <f t="shared" si="75"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" si="76"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z42" t="str">
-        <f t="shared" si="77"/>
-        <v>{"user":"lorenz-haenggi","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>49</v>
@@ -6211,64 +6211,64 @@
         <v>{</v>
       </c>
       <c r="N43" t="str">
-        <f t="shared" ref="N43" si="78">IF(N$4=0,M43,M43&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A43&amp;"""",IF(N$3=2,IF(A43=1,"true", "false"),A43))&amp;IF(ISBLANK(O$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O43" t="str">
-        <f t="shared" ref="O43" si="79">IF(O$4=0,N43,N43&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B43&amp;"""",IF(O$3=2,IF(B43=1,"true", "false"),B43))&amp;IF(ISBLANK(P$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub"</v>
       </c>
       <c r="P43" t="str">
-        <f t="shared" ref="P43" si="80">IF(P$4=0,O43,O43&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C43&amp;"""",IF(P$3=2,IF(C43=1,"true", "false"),C43))&amp;IF(ISBLANK(Q$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":""</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" ref="Q43" si="81">IF(Q$4=0,P43,P43&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D43&amp;"""",IF(Q$3=2,IF(D43=1,"true", "false"),D43))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" ref="R43" si="82">IF(R$4=0,Q43,Q43&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E43&amp;"""",IF(R$3=2,IF(E43=1,"true", "false"),E43))&amp;IF(ISBLANK(S$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S43" t="str">
-        <f t="shared" ref="S43" si="83">IF(S$4=0,R43,R43&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F43&amp;"""",IF(S$3=2,IF(F43=1,"true", "false"),F43))&amp;IF(ISBLANK(T$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" ref="T43" si="84">IF(T$4=0,S43,S43&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G43&amp;"""",IF(T$3=2,IF(G43=1,"true", "false"),G43))&amp;IF(ISBLANK(U$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U43" t="str">
-        <f t="shared" ref="U43" si="85">IF(U$4=0,T43,T43&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H43&amp;"""",IF(U$3=2,IF(H43=1,"true", "false"),H43))&amp;IF(ISBLANK(V$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V43" t="str">
-        <f t="shared" ref="V43" si="86">IF(V$4=0,U43,U43&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I43&amp;"""",IF(V$3=2,IF(I43=1,"true", "false"),I43))&amp;IF(ISBLANK(W$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W43" t="str">
-        <f t="shared" ref="W43" si="87">IF(W$4=0,V43,V43&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J43&amp;"""",IF(W$3=2,IF(J43=1,"true", "false"),J43))&amp;IF(ISBLANK(X$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X43" t="str">
-        <f t="shared" ref="X43" si="88">IF(X$4=0,W43,W43&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K43&amp;"""",IF(X$3=2,IF(K43=1,"true", "false"),K43))&amp;IF(ISBLANK(Y$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y43" t="str">
-        <f t="shared" ref="Y43" si="89">IF(Y$4=0,X43,X43&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L43&amp;"""",IF(Y$3=2,IF(L43=1,"true", "false"),L43))&amp;IF(ISBLANK(Z$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z43" t="str">
-        <f t="shared" ref="Z43" si="90">IF(ISBLANK(A43),"",Y43&amp;"}"&amp;IF(OR(Z44="]",Z44="",ISBLANK(Z44)),"",","))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>49</v>
@@ -6287,56 +6287,56 @@
         <v>{</v>
       </c>
       <c r="N44" t="str">
-        <f t="shared" ref="N44:N56" si="91">IF(N$4=0,M44,M44&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A44&amp;"""",IF(N$3=2,IF(A44=1,"true", "false"),A44))&amp;IF(ISBLANK(O$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi"</v>
+        <f t="shared" si="4"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="O44" t="str">
-        <f t="shared" ref="O44:O56" si="92">IF(O$4=0,N44,N44&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B44&amp;"""",IF(O$3=2,IF(B44=1,"true", "false"),B44))&amp;IF(ISBLANK(P$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Todesfall"</v>
       </c>
       <c r="P44" t="str">
-        <f t="shared" ref="P44:P56" si="93">IF(P$4=0,O44,O44&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C44&amp;"""",IF(P$3=2,IF(C44=1,"true", "false"),C44))&amp;IF(ISBLANK(Q$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Todesfall","text":""</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" ref="Q44:Q56" si="94">IF(Q$4=0,P44,P44&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D44&amp;"""",IF(Q$3=2,IF(D44=1,"true", "false"),D44))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" ref="R44:R56" si="95">IF(R$4=0,Q44,Q44&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E44&amp;"""",IF(R$3=2,IF(E44=1,"true", "false"),E44))&amp;IF(ISBLANK(S$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S44" t="str">
-        <f t="shared" ref="S44:S56" si="96">IF(S$4=0,R44,R44&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F44&amp;"""",IF(S$3=2,IF(F44=1,"true", "false"),F44))&amp;IF(ISBLANK(T$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" ref="T44:T56" si="97">IF(T$4=0,S44,S44&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G44&amp;"""",IF(T$3=2,IF(G44=1,"true", "false"),G44))&amp;IF(ISBLANK(U$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U44" t="str">
-        <f t="shared" ref="U44:U56" si="98">IF(U$4=0,T44,T44&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H44&amp;"""",IF(U$3=2,IF(H44=1,"true", "false"),H44))&amp;IF(ISBLANK(V$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V44" t="str">
-        <f t="shared" ref="V44:V56" si="99">IF(V$4=0,U44,U44&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I44&amp;"""",IF(V$3=2,IF(I44=1,"true", "false"),I44))&amp;IF(ISBLANK(W$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W44" t="str">
-        <f t="shared" ref="W44:W56" si="100">IF(W$4=0,V44,V44&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J44&amp;"""",IF(W$3=2,IF(J44=1,"true", "false"),J44))&amp;IF(ISBLANK(X$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X44" t="str">
-        <f t="shared" ref="X44:X56" si="101">IF(X$4=0,W44,W44&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K44&amp;"""",IF(X$3=2,IF(K44=1,"true", "false"),K44))&amp;IF(ISBLANK(Y$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y44" t="str">
-        <f t="shared" ref="Y44:Y56" si="102">IF(Y$4=0,X44,X44&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L44&amp;"""",IF(Y$3=2,IF(L44=1,"true", "false"),L44))&amp;IF(ISBLANK(Z$3),"},",""))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z44" t="str">
-        <f t="shared" ref="Z44:Z56" si="103">IF(ISBLANK(A44),"",Y44&amp;"}"&amp;IF(OR(Z45="]",Z45="",ISBLANK(Z45)),"",","))</f>
-        <v>{"user":"lorenz-haenggi","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="12"/>
+        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
@@ -6344,7 +6344,7 @@
         <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>49</v>
@@ -6363,968 +6363,800 @@
         <v>{</v>
       </c>
       <c r="N45" t="str">
-        <f t="shared" si="91"/>
+        <f t="shared" si="4"/>
         <v>{"user":"User"</v>
       </c>
       <c r="O45" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Wohnungswechsel"</v>
+        <f t="shared" si="5"/>
+        <v>{"user":"User","typ":"Kompensation"</v>
       </c>
       <c r="P45" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":""</v>
+        <f t="shared" si="6"/>
+        <v>{"user":"User","typ":"Kompensation","text":""</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="7"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15"</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="8"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
       </c>
       <c r="S45" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="9"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="10"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="U45" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="39"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="V45" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="40"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="W45" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="41"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="X45" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="42"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Y45" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="43"/>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
       </c>
       <c r="Z45" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Wohnungswechsel","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f>IF(ISBLANK(A45),"",Y45&amp;"}"&amp;IF(OR(Z46="]",Z46="",ISBLANK(Z46)),"",","))</f>
+        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false}</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F46">
-        <v>3</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>53</v>
-      </c>
+    <row r="46" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="G46" s="5"/>
       <c r="M46" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N46" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" ref="N46:N56" si="44">IF(N$4=0,M46,M46&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A46&amp;"""",IF(N$3=2,IF(A46=1,"true", "false"),A46))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":""</v>
       </c>
       <c r="O46" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Kurs"</v>
+        <f t="shared" ref="O46:O56" si="45">IF(O$4=0,N46,N46&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B46&amp;"""",IF(O$3=2,IF(B46=1,"true", "false"),B46))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P46" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Kurs","text":""</v>
+        <f t="shared" ref="P46:P56" si="46">IF(P$4=0,O46,O46&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C46&amp;"""",IF(P$3=2,IF(C46=1,"true", "false"),C46))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" ref="Q46:Q56" si="47">IF(Q$4=0,P46,P46&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D46&amp;"""",IF(Q$3=2,IF(D46=1,"true", "false"),D46))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" ref="R46:R56" si="48">IF(R$4=0,Q46,Q46&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E46&amp;"""",IF(R$3=2,IF(E46=1,"true", "false"),E46))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" ref="S46:S56" si="49">IF(S$4=0,R46,R46&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F46&amp;"""",IF(S$3=2,IF(F46=1,"true", "false"),F46))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="T46:T56" si="50">IF(T$4=0,S46,S46&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G46&amp;"""",IF(T$3=2,IF(G46=1,"true", "false"),G46))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U46" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="U46:U56" si="51">IF(U$4=0,T46,T46&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H46&amp;"""",IF(U$3=2,IF(H46=1,"true", "false"),H46))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V46" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="V46:V56" si="52">IF(V$4=0,U46,U46&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I46&amp;"""",IF(V$3=2,IF(I46=1,"true", "false"),I46))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W46" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="W46:W56" si="53">IF(W$4=0,V46,V46&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J46&amp;"""",IF(W$3=2,IF(J46=1,"true", "false"),J46))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X46" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="X46:X56" si="54">IF(X$4=0,W46,W46&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K46&amp;"""",IF(X$3=2,IF(K46=1,"true", "false"),K46))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="Y46:Y56" si="55">IF(Y$4=0,X46,X46&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L46&amp;"""",IF(Y$3=2,IF(L46=1,"true", "false"),L46))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z46" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Kurs","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" ref="Z46:Z56" si="56">IF(ISBLANK(A46),"",Y46&amp;"}"&amp;IF(OR(Z47="]",Z47="",ISBLANK(Z47)),"",","))</f>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F47">
-        <v>3</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A47" s="11"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="G47" s="5"/>
       <c r="M47" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N47" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O47" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Unfall"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P47" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Unfall","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R47" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S47" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U47" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V47" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W47" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X47" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y47" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z47" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Unfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48">
-        <v>3</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A48" s="11"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="G48" s="5"/>
       <c r="M48" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N48" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O48" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Ferien"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P48" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Ferien","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R48" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S48" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U48" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V48" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W48" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X48" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y48" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z48" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Ferien","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" t="s">
-        <v>59</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F49">
-        <v>3</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A49" s="11"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="G49" s="5"/>
       <c r="M49" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N49" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O49" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Krankheit"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Krankheit","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q49" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R49" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S49" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U49" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V49" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W49" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X49" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y49" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z49" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Krankheit","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" t="s">
-        <v>66</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F50">
-        <v>3</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A50" s="11"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="G50" s="5"/>
       <c r="M50" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N50" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O50" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Heirat"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P50" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Heirat","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S50" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U50" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V50" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W50" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X50" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y50" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z50" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Heirat","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F51">
-        <v>3</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A51" s="11"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="G51" s="5"/>
       <c r="M51" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N51" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O51" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Jubiläum"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P51" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Jubiläum","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S51" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U51" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V51" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W51" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X51" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y51" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z51" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Jubiläum","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F52">
-        <v>3</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A52" s="11"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="G52" s="5"/>
       <c r="M52" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N52" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O52" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P52" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R52" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S52" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T52" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U52" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V52" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W52" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X52" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y52" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z52" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Mutterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F53">
-        <v>3</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A53" s="11"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="G53" s="5"/>
       <c r="M53" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N53" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O53" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R53" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S53" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U53" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V53" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W53" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X53" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y53" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z53" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Militär+Zivilschutz","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54">
-        <v>3</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A54" s="11"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="G54" s="5"/>
       <c r="M54" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O54" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Unbezahlt"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R54" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S54" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U54" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V54" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W54" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X54" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y54" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z54" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Unbezahlt","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" t="s">
-        <v>54</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F55">
-        <v>3</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A55" s="11"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="G55" s="5"/>
       <c r="M55" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N55" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O55" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q55" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R55" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S55" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T55" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U55" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V55" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W55" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X55" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y55" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z55" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Vaterschaftsurlaub","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" t="s">
-        <v>71</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F56">
-        <v>3</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A56" s="11"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="G56" s="5"/>
       <c r="M56" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N56" t="str">
-        <f t="shared" si="91"/>
-        <v>{"user":"User"</v>
+        <f t="shared" si="44"/>
+        <v>{"user":""</v>
       </c>
       <c r="O56" t="str">
-        <f t="shared" si="92"/>
-        <v>{"user":"User","typ":"Todesfall"</v>
+        <f t="shared" si="45"/>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P56" t="str">
-        <f t="shared" si="93"/>
-        <v>{"user":"User","typ":"Todesfall","text":""</v>
+        <f t="shared" si="46"/>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q56" t="str">
-        <f t="shared" si="94"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" si="47"/>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R56" t="str">
-        <f t="shared" si="95"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" si="48"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S56" t="str">
-        <f t="shared" si="96"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" si="49"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T56" t="str">
-        <f t="shared" si="97"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="50"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U56" t="str">
-        <f t="shared" si="98"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="51"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V56" t="str">
-        <f t="shared" si="99"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="52"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W56" t="str">
-        <f t="shared" si="100"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="53"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X56" t="str">
-        <f t="shared" si="101"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="54"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y56" t="str">
-        <f t="shared" si="102"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" si="55"/>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z56" t="str">
-        <f t="shared" si="103"/>
-        <v>{"user":"User","typ":"Todesfall","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false},</v>
+        <f t="shared" si="56"/>
+        <v/>
       </c>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F57">
-        <v>3</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A57" s="11"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="G57" s="5"/>
       <c r="M57" t="str">
         <f t="shared" si="3"/>
         <v>{</v>
       </c>
       <c r="N57" t="str">
-        <f t="shared" ref="N57" si="104">IF(N$4=0,M57,M57&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A57&amp;"""",IF(N$3=2,IF(A57=1,"true", "false"),A57))&amp;IF(ISBLANK(O$3),"},",""))</f>
-        <v>{"user":"User"</v>
+        <f t="shared" ref="N57" si="57">IF(N$4=0,M57,M57&amp;IF(ISBLANK(M$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(N$3=1,""""&amp;A57&amp;"""",IF(N$3=2,IF(A57=1,"true", "false"),A57))&amp;IF(ISBLANK(O$3),"},",""))</f>
+        <v>{"user":""</v>
       </c>
       <c r="O57" t="str">
-        <f t="shared" ref="O57" si="105">IF(O$4=0,N57,N57&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B57&amp;"""",IF(O$3=2,IF(B57=1,"true", "false"),B57))&amp;IF(ISBLANK(P$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation"</v>
+        <f t="shared" ref="O57" si="58">IF(O$4=0,N57,N57&amp;IF(ISBLANK(N$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(O$3=1,""""&amp;B57&amp;"""",IF(O$3=2,IF(B57=1,"true", "false"),B57))&amp;IF(ISBLANK(P$3),"},",""))</f>
+        <v>{"user":"","typ":""</v>
       </c>
       <c r="P57" t="str">
-        <f t="shared" ref="P57" si="106">IF(P$4=0,O57,O57&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C57&amp;"""",IF(P$3=2,IF(C57=1,"true", "false"),C57))&amp;IF(ISBLANK(Q$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":""</v>
+        <f t="shared" ref="P57" si="59">IF(P$4=0,O57,O57&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;C$4&amp;""":"&amp;IF(P$3=1,""""&amp;C57&amp;"""",IF(P$3=2,IF(C57=1,"true", "false"),C57))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":""</v>
       </c>
       <c r="Q57" t="str">
-        <f t="shared" ref="Q57" si="107">IF(Q$4=0,P57,P57&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D57&amp;"""",IF(Q$3=2,IF(D57=1,"true", "false"),D57))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15"</v>
+        <f t="shared" ref="Q57" si="60">IF(Q$4=0,P57,P57&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;D$4&amp;""":"&amp;IF(Q$3=1,""""&amp;D57&amp;"""",IF(Q$3=2,IF(D57=1,"true", "false"),D57))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":""</v>
       </c>
       <c r="R57" t="str">
-        <f t="shared" ref="R57" si="108">IF(R$4=0,Q57,Q57&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E57&amp;"""",IF(R$3=2,IF(E57=1,"true", "false"),E57))&amp;IF(ISBLANK(S$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18"</v>
+        <f t="shared" ref="R57" si="61">IF(R$4=0,Q57,Q57&amp;IF(ISBLANK(Q$3),"",",")&amp;""""&amp;E$4&amp;""":"&amp;IF(R$3=1,""""&amp;E57&amp;"""",IF(R$3=2,IF(E57=1,"true", "false"),E57))&amp;IF(ISBLANK(S$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":""</v>
       </c>
       <c r="S57" t="str">
-        <f t="shared" ref="S57" si="109">IF(S$4=0,R57,R57&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F57&amp;"""",IF(S$3=2,IF(F57=1,"true", "false"),F57))&amp;IF(ISBLANK(T$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3</v>
+        <f t="shared" ref="S57" si="62">IF(S$4=0,R57,R57&amp;IF(ISBLANK(R$3),"",",")&amp;""""&amp;F$4&amp;""":"&amp;IF(S$3=1,""""&amp;F57&amp;"""",IF(S$3=2,IF(F57=1,"true", "false"),F57))&amp;IF(ISBLANK(T$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":</v>
       </c>
       <c r="T57" t="str">
-        <f t="shared" ref="T57" si="110">IF(T$4=0,S57,S57&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G57&amp;"""",IF(T$3=2,IF(G57=1,"true", "false"),G57))&amp;IF(ISBLANK(U$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="T57" si="63">IF(T$4=0,S57,S57&amp;IF(ISBLANK(S$3),"",",")&amp;""""&amp;G$4&amp;""":"&amp;IF(T$3=1,""""&amp;G57&amp;"""",IF(T$3=2,IF(G57=1,"true", "false"),G57))&amp;IF(ISBLANK(U$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="U57" t="str">
-        <f t="shared" ref="U57" si="111">IF(U$4=0,T57,T57&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H57&amp;"""",IF(U$3=2,IF(H57=1,"true", "false"),H57))&amp;IF(ISBLANK(V$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="U57" si="64">IF(U$4=0,T57,T57&amp;IF(ISBLANK(T$3),"",",")&amp;""""&amp;H$4&amp;""":"&amp;IF(U$3=1,""""&amp;H57&amp;"""",IF(U$3=2,IF(H57=1,"true", "false"),H57))&amp;IF(ISBLANK(V$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="V57" t="str">
-        <f t="shared" ref="V57" si="112">IF(V$4=0,U57,U57&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I57&amp;"""",IF(V$3=2,IF(I57=1,"true", "false"),I57))&amp;IF(ISBLANK(W$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="V57" si="65">IF(V$4=0,U57,U57&amp;IF(ISBLANK(U$3),"",",")&amp;""""&amp;I$4&amp;""":"&amp;IF(V$3=1,""""&amp;I57&amp;"""",IF(V$3=2,IF(I57=1,"true", "false"),I57))&amp;IF(ISBLANK(W$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="W57" t="str">
-        <f t="shared" ref="W57" si="113">IF(W$4=0,V57,V57&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J57&amp;"""",IF(W$3=2,IF(J57=1,"true", "false"),J57))&amp;IF(ISBLANK(X$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="W57" si="66">IF(W$4=0,V57,V57&amp;IF(ISBLANK(V$3),"",",")&amp;""""&amp;J$4&amp;""":"&amp;IF(W$3=1,""""&amp;J57&amp;"""",IF(W$3=2,IF(J57=1,"true", "false"),J57))&amp;IF(ISBLANK(X$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="X57" t="str">
-        <f t="shared" ref="X57" si="114">IF(X$4=0,W57,W57&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K57&amp;"""",IF(X$3=2,IF(K57=1,"true", "false"),K57))&amp;IF(ISBLANK(Y$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="X57" si="67">IF(X$4=0,W57,W57&amp;IF(ISBLANK(W$3),"",",")&amp;""""&amp;K$4&amp;""":"&amp;IF(X$3=1,""""&amp;K57&amp;"""",IF(X$3=2,IF(K57=1,"true", "false"),K57))&amp;IF(ISBLANK(Y$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Y57" t="str">
-        <f t="shared" ref="Y57" si="115">IF(Y$4=0,X57,X57&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L57&amp;"""",IF(Y$3=2,IF(L57=1,"true", "false"),L57))&amp;IF(ISBLANK(Z$3),"},",""))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false</v>
+        <f t="shared" ref="Y57" si="68">IF(Y$4=0,X57,X57&amp;IF(ISBLANK(X$3),"",",")&amp;""""&amp;L$4&amp;""":"&amp;IF(Y$3=1,""""&amp;L57&amp;"""",IF(Y$3=2,IF(L57=1,"true", "false"),L57))&amp;IF(ISBLANK(Z$3),"},",""))</f>
+        <v>{"user":"","typ":"","text":"","fromDate":"","toDate":"","days":,"commit":</v>
       </c>
       <c r="Z57" t="str">
-        <f t="shared" ref="Z57" si="116">IF(ISBLANK(A57),"",Y57&amp;"}"&amp;IF(OR(Z58="]",Z58="",ISBLANK(Z58)),"",","))</f>
-        <v>{"user":"User","typ":"Kompensation","text":"","fromDate":"2017-02-15","toDate":"2017-02-18","days":3,"commit":false}</v>
+        <f t="shared" ref="Z57" si="69">IF(ISBLANK(A57),"",Y57&amp;"}"&amp;IF(OR(Z58="]",Z58="",ISBLANK(Z58)),"",","))</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>